<commit_message>
Add user creation and email/password generator modules
Added modules for automated user creation in Office 365 and AppConnecto, including email and password generators. Enhanced AppConnecto automation with debug screenshot support and improved error handling. Updated configuration for default values and group mappings. Extended Graph API client with user/group management utilities. Added tests and updated requirements.
</commit_message>
<xml_diff>
--- a/Solicitud correos prueba.xlsx
+++ b/Solicitud correos prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecrcampus-my.sharepoint.com/personal/carlos_perezc_ecr_edu_co/Documents/Backup ECR Tecnologia/Documents/GitHub/UserAutomationService/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1433097B-FBD3-4C4A-A257-93A66F85079C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{1433097B-FBD3-4C4A-A257-93A66F85079C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D9BEAC4-2F32-421A-9385-49264A31B452}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="RlsOItVjzIoOeYUFU/eLw5DQouYEYDvsGdSxxjpsn7Vqy/bWq+hBVjSLC/Rv1KTSkLjsk4SBD6qU7dIN8cKa0Q==" workbookSaltValue="wbbWpA/jt21F3SOY0vH1TQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="119">
   <si>
     <t>Escuela Colombiana de Rehabilitación</t>
   </si>
@@ -365,9 +365,6 @@
     <t>SEBASTIAN ORLANDO</t>
   </si>
   <si>
-    <t>ANDRÉS MATEO</t>
-  </si>
-  <si>
     <t>AMAYA ZÚÑIGA</t>
   </si>
   <si>
@@ -389,9 +386,6 @@
     <t>RODRIGUEZ NIVIA</t>
   </si>
   <si>
-    <t>RODRÍGUEZ RIVERA</t>
-  </si>
-  <si>
     <t>ESPECIALIZACIÓN EN TERAPIA MANUAL  (610 )</t>
   </si>
   <si>
@@ -416,9 +410,6 @@
     <t>vanessarodriguez@ecr.edu.co</t>
   </si>
   <si>
-    <t>marori1108@gmail.com</t>
-  </si>
-  <si>
     <t>C.C</t>
   </si>
   <si>
@@ -426,13 +417,67 @@
   </si>
   <si>
     <t>Apellido</t>
+  </si>
+  <si>
+    <t>ezio auditore</t>
+  </si>
+  <si>
+    <t>Firenze</t>
+  </si>
+  <si>
+    <t>ezioauditore@gmail.com</t>
+  </si>
+  <si>
+    <t>Nicolás</t>
+  </si>
+  <si>
+    <t>Maquiavelo</t>
+  </si>
+  <si>
+    <t>nicolasmaquiavelo@gmail.com</t>
+  </si>
+  <si>
+    <t>Michelangelo</t>
+  </si>
+  <si>
+    <t>Buonarroti</t>
+  </si>
+  <si>
+    <t>michelangelobuonarroti@gmail.com</t>
+  </si>
+  <si>
+    <t>Dante</t>
+  </si>
+  <si>
+    <t>Inferno</t>
+  </si>
+  <si>
+    <t>danteinferno@gmail.com</t>
+  </si>
+  <si>
+    <t>Sandro</t>
+  </si>
+  <si>
+    <t>Botticelli</t>
+  </si>
+  <si>
+    <t>sandrobotticelli@gmail.com</t>
+  </si>
+  <si>
+    <t>Galileo</t>
+  </si>
+  <si>
+    <t>Galilei</t>
+  </si>
+  <si>
+    <t>galileogalilei@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,6 +561,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -697,7 +750,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -779,6 +832,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -808,12 +871,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -898,6 +955,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1166,11 +1227,11 @@
   <sheetPr codeName="Hoja1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1198,15 +1259,15 @@
     <col min="21" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>3</v>
@@ -1217,7 +1278,7 @@
       <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="28" t="s">
@@ -1247,7 +1308,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E2" s="16">
         <v>1000227618</v>
@@ -1285,7 +1346,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E3" s="16">
         <v>1000214175</v>
@@ -1323,7 +1384,7 @@
         <v>60</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E4" s="16">
         <v>1000373017</v>
@@ -1361,7 +1422,7 @@
         <v>61</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E5" s="16">
         <v>1010034368</v>
@@ -1399,7 +1460,7 @@
         <v>62</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E6" s="16">
         <v>1002634900</v>
@@ -1437,7 +1498,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E7" s="16">
         <v>1019066112</v>
@@ -1475,7 +1536,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E8" s="16">
         <v>1003479182</v>
@@ -1513,7 +1574,7 @@
         <v>65</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E9" s="16">
         <v>1140836363</v>
@@ -1551,7 +1612,7 @@
         <v>66</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E10" s="16">
         <v>1007696307</v>
@@ -1586,10 +1647,10 @@
         <v>77</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E11" s="16">
         <v>38600274</v>
@@ -1598,10 +1659,10 @@
         <v>11</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1624,10 +1685,10 @@
         <v>78</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E12" s="16">
         <v>1014295995</v>
@@ -1636,10 +1697,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="24" t="s">
         <v>92</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>94</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1662,10 +1723,10 @@
         <v>79</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E13" s="16">
         <v>1000506141</v>
@@ -1674,10 +1735,10 @@
         <v>11</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
@@ -1700,10 +1761,10 @@
         <v>80</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E14" s="16">
         <v>45521464</v>
@@ -1712,10 +1773,10 @@
         <v>11</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1738,10 +1799,10 @@
         <v>81</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E15" s="16">
         <v>1053611435</v>
@@ -1750,10 +1811,10 @@
         <v>11</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -1776,10 +1837,10 @@
         <v>82</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E16" s="16">
         <v>1010029988</v>
@@ -1788,10 +1849,10 @@
         <v>11</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -1814,10 +1875,10 @@
         <v>80</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E17" s="16">
         <v>1019104024</v>
@@ -1826,10 +1887,10 @@
         <v>11</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -1849,25 +1910,25 @@
         <v>34</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E18" s="16">
-        <v>1003635469</v>
+        <v>1000000001</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>100</v>
+        <v>90</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>103</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
@@ -1882,21 +1943,217 @@
       <c r="S18"/>
       <c r="T18"/>
     </row>
+    <row r="19" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1000000002</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+    </row>
+    <row r="20" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1000000003</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+    </row>
+    <row r="21" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="16">
+        <v>1000000004</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+    </row>
+    <row r="22" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="16">
+        <v>1000000005</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+    </row>
+    <row r="23" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1000000006</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E19:E1048576 E1">
+  <conditionalFormatting sqref="E24:E1048576 E1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18" xr:uid="{AD4AA420-3D35-43F9-9FA5-1C49A677BF2D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D23" xr:uid="{AD4AA420-3D35-43F9-9FA5-1C49A677BF2D}">
       <formula1>"  C.C,C.E"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="H14" r:id="rId1" xr:uid="{7FB6ED01-29A3-429D-800C-35964F7AA868}"/>
+    <hyperlink ref="H19" r:id="rId2" xr:uid="{954CC9C7-1400-4CDB-B940-AD32EF416845}"/>
+    <hyperlink ref="H18" r:id="rId3" xr:uid="{7536DEE8-064B-40AA-B689-65B08B66B015}"/>
+    <hyperlink ref="H20" r:id="rId4" xr:uid="{528E2B77-B679-4197-A5DC-C760C3A1FC6F}"/>
+    <hyperlink ref="H21" r:id="rId5" xr:uid="{FFC5DFBF-96D6-4958-B2C1-6CE7C345AEE1}"/>
+    <hyperlink ref="H22" r:id="rId6" xr:uid="{2216D0DB-0C1D-4AC2-AA74-11ED5C4BE61A}"/>
+    <hyperlink ref="H23" r:id="rId7" xr:uid="{579B0E13-F803-480F-AAF1-5CBF8DFDDFAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1904,13 +2161,13 @@
           <x14:formula1>
             <xm:f>Hoja2!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F18</xm:sqref>
+          <xm:sqref>F2:F23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Hoja2!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A18</xm:sqref>
+          <xm:sqref>A2:A23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1963,73 +2220,73 @@
       <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="32"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="36"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="39" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="35"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="40" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="31"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="41"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="39" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="35"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="40" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="38"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="41"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -2037,34 +2294,34 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="31"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="40" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="41"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="38"/>
     </row>
     <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">

</xml_diff>

<commit_message>
Add email sending automation and welcome email template
Introduces automated welcome email sending using Microsoft Graph API and Jinja2 templates. Adds EmailSender class, welcome_email.html template, and supporting test script. Updates config to support email settings, adds requirements for Jinja2, and implements email sending in the main automation workflow. Also restructures main.py and updates AppConnecto and Office 365 user creation flow.
</commit_message>
<xml_diff>
--- a/Solicitud correos prueba.xlsx
+++ b/Solicitud correos prueba.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecrcampus-my.sharepoint.com/personal/carlos_perezc_ecr_edu_co/Documents/Backup ECR Tecnologia/Documents/GitHub/UserAutomationService/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{1433097B-FBD3-4C4A-A257-93A66F85079C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D9BEAC4-2F32-421A-9385-49264A31B452}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{1433097B-FBD3-4C4A-A257-93A66F85079C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B17BC385-8C02-4DB4-8A53-2335586956AE}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="RlsOItVjzIoOeYUFU/eLw5DQouYEYDvsGdSxxjpsn7Vqy/bWq+hBVjSLC/Rv1KTSkLjsk4SBD6qU7dIN8cKa0Q==" workbookSaltValue="wbbWpA/jt21F3SOY0vH1TQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
   <si>
     <t>Escuela Colombiana de Rehabilitación</t>
   </si>
@@ -452,25 +452,25 @@
     <t>Inferno</t>
   </si>
   <si>
-    <t>danteinferno@gmail.com</t>
-  </si>
-  <si>
     <t>Sandro</t>
   </si>
   <si>
     <t>Botticelli</t>
   </si>
   <si>
-    <t>sandrobotticelli@gmail.com</t>
-  </si>
-  <si>
     <t>Galileo</t>
   </si>
   <si>
     <t>Galilei</t>
   </si>
   <si>
-    <t>galileogalilei@gmail.com</t>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>carpeca1998@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -1227,11 +1227,11 @@
   <sheetPr codeName="Hoja1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2033,7 +2033,7 @@
         <v>98</v>
       </c>
       <c r="E21" s="16">
-        <v>1000000004</v>
+        <v>1000000014</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>11</v>
@@ -2042,7 +2042,7 @@
         <v>90</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
@@ -2062,16 +2062,16 @@
         <v>34</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>113</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>114</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>98</v>
       </c>
       <c r="E22" s="16">
-        <v>1000000005</v>
+        <v>1000000015</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>11</v>
@@ -2080,7 +2080,7 @@
         <v>90</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -2100,16 +2100,16 @@
         <v>34</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>98</v>
       </c>
       <c r="E23" s="16">
-        <v>1000000006</v>
+        <v>1000000016</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>11</v>
@@ -2133,12 +2133,50 @@
       <c r="S23"/>
       <c r="T23"/>
     </row>
+    <row r="24" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="16">
+        <v>1000000017</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E24:E1048576 E1">
+  <conditionalFormatting sqref="E25:E1048576 E1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D23" xr:uid="{AD4AA420-3D35-43F9-9FA5-1C49A677BF2D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D24" xr:uid="{AD4AA420-3D35-43F9-9FA5-1C49A677BF2D}">
       <formula1>"  C.C,C.E"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2150,10 +2188,11 @@
     <hyperlink ref="H21" r:id="rId5" xr:uid="{FFC5DFBF-96D6-4958-B2C1-6CE7C345AEE1}"/>
     <hyperlink ref="H22" r:id="rId6" xr:uid="{2216D0DB-0C1D-4AC2-AA74-11ED5C4BE61A}"/>
     <hyperlink ref="H23" r:id="rId7" xr:uid="{579B0E13-F803-480F-AAF1-5CBF8DFDDFAC}"/>
+    <hyperlink ref="H24" r:id="rId8" xr:uid="{303A75CB-2E69-4046-940D-682C6608DDEA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
-  <legacyDrawing r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -2161,13 +2200,13 @@
           <x14:formula1>
             <xm:f>Hoja2!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F23</xm:sqref>
+          <xm:sqref>F2:F24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Hoja2!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A23</xm:sqref>
+          <xm:sqref>A2:A24</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2577,17 +2616,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fe812fb7-574b-44ed-86d0-2d16146268c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="37e87451-74b3-4048-bfb9-7d04c800d92b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F857DE7301CF354A96FB0056A5C63AD9" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="43c9f770e0b755e4ff9e568834e2ba42">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe812fb7-574b-44ed-86d0-2d16146268c6" xmlns:ns3="37e87451-74b3-4048-bfb9-7d04c800d92b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd07d1d3ab751488f84a45fcf1374d77" ns2:_="" ns3:_="">
     <xsd:import namespace="fe812fb7-574b-44ed-86d0-2d16146268c6"/>
@@ -2788,6 +2816,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fe812fb7-574b-44ed-86d0-2d16146268c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="37e87451-74b3-4048-bfb9-7d04c800d92b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{427495A4-75F5-4F6F-B663-AAB6EE1BCE95}">
   <ds:schemaRefs>
@@ -2797,17 +2836,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46325D9C-2D75-4F78-B099-4FB167734A1F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fe812fb7-574b-44ed-86d0-2d16146268c6"/>
-    <ds:schemaRef ds:uri="37e87451-74b3-4048-bfb9-7d04c800d92b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8866EC1-C81B-4E43-AC87-31312149C8C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2824,4 +2852,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46325D9C-2D75-4F78-B099-4FB167734A1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fe812fb7-574b-44ed-86d0-2d16146268c6"/>
+    <ds:schemaRef ds:uri="37e87451-74b3-4048-bfb9-7d04c800d92b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add PDF and Excel report generation
Introduces a new ReportGenerator class to create detailed PDF and Excel reports of the user automation process. Updates main.py to generate these reports at the end of the workflow, even if no new users are processed. Adds documentation (GUIA_REPORTES.md) describing report formats and usage. Updates requirements.txt to include reportlab and openpyxl dependencies.
</commit_message>
<xml_diff>
--- a/Solicitud correos prueba.xlsx
+++ b/Solicitud correos prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecrcampus-my.sharepoint.com/personal/carlos_perezc_ecr_edu_co/Documents/Backup ECR Tecnologia/Documents/GitHub/UserAutomationService/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{1433097B-FBD3-4C4A-A257-93A66F85079C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B17BC385-8C02-4DB4-8A53-2335586956AE}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{1433097B-FBD3-4C4A-A257-93A66F85079C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36DA69E2-8D6E-4206-B1DE-D5AE7F24996E}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="RlsOItVjzIoOeYUFU/eLw5DQouYEYDvsGdSxxjpsn7Vqy/bWq+hBVjSLC/Rv1KTSkLjsk4SBD6qU7dIN8cKa0Q==" workbookSaltValue="wbbWpA/jt21F3SOY0vH1TQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="121">
   <si>
     <t>Escuela Colombiana de Rehabilitación</t>
   </si>
@@ -471,6 +471,12 @@
   </si>
   <si>
     <t>carpeca1998@hotmail.com</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Borgia</t>
   </si>
 </sst>
 </file>
@@ -1227,11 +1233,11 @@
   <sheetPr codeName="Hoja1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C19" sqref="C19"/>
+      <selection pane="topRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2171,12 +2177,50 @@
       <c r="S24"/>
       <c r="T24"/>
     </row>
+    <row r="25" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="16">
+        <v>1000000018</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E25:E1048576 E1">
+  <conditionalFormatting sqref="E26:E1048576 E1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D24" xr:uid="{AD4AA420-3D35-43F9-9FA5-1C49A677BF2D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D25" xr:uid="{AD4AA420-3D35-43F9-9FA5-1C49A677BF2D}">
       <formula1>"  C.C,C.E"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2189,10 +2233,11 @@
     <hyperlink ref="H22" r:id="rId6" xr:uid="{2216D0DB-0C1D-4AC2-AA74-11ED5C4BE61A}"/>
     <hyperlink ref="H23" r:id="rId7" xr:uid="{579B0E13-F803-480F-AAF1-5CBF8DFDDFAC}"/>
     <hyperlink ref="H24" r:id="rId8" xr:uid="{303A75CB-2E69-4046-940D-682C6608DDEA}"/>
+    <hyperlink ref="H25" r:id="rId9" xr:uid="{C81B15B4-CBA4-402E-ABE7-9F9DD770DC17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -2200,13 +2245,13 @@
           <x14:formula1>
             <xm:f>Hoja2!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F24</xm:sqref>
+          <xm:sqref>F2:F25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Hoja2!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A24</xm:sqref>
+          <xm:sqref>A2:A25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2607,12 +2652,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fe812fb7-574b-44ed-86d0-2d16146268c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="37e87451-74b3-4048-bfb9-7d04c800d92b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2817,20 +2864,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fe812fb7-574b-44ed-86d0-2d16146268c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="37e87451-74b3-4048-bfb9-7d04c800d92b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{427495A4-75F5-4F6F-B663-AAB6EE1BCE95}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46325D9C-2D75-4F78-B099-4FB167734A1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fe812fb7-574b-44ed-86d0-2d16146268c6"/>
+    <ds:schemaRef ds:uri="37e87451-74b3-4048-bfb9-7d04c800d92b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2855,12 +2903,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46325D9C-2D75-4F78-B099-4FB167734A1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{427495A4-75F5-4F6F-B663-AAB6EE1BCE95}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fe812fb7-574b-44ed-86d0-2d16146268c6"/>
-    <ds:schemaRef ds:uri="37e87451-74b3-4048-bfb9-7d04c800d92b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>